<commit_message>
refactored code, organised folders, modularised code
</commit_message>
<xml_diff>
--- a/data/meals.xlsx
+++ b/data/meals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A16D1E5-44B3-44EB-8194-8C5E179BC276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C17AF7-E6B9-498A-92A0-512A0016B0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>recipe_name</t>
   </si>
@@ -123,9 +123,6 @@
     <t>miso, dashi, noodles,</t>
   </si>
   <si>
-    <t>couscous, aubergine,</t>
-  </si>
-  <si>
     <t>rice, coconut milk,</t>
   </si>
   <si>
@@ -181,6 +178,12 @@
   </si>
   <si>
     <t>chicken_wings,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couscous, </t>
+  </si>
+  <si>
+    <t>aubergine,</t>
   </si>
 </sst>
 </file>
@@ -517,9 +520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -629,7 +632,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.3">
@@ -637,7 +640,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -648,7 +651,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
@@ -659,7 +662,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>19</v>
@@ -667,10 +670,10 @@
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>
@@ -681,10 +684,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.3">
@@ -692,13 +698,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.3">
@@ -717,7 +723,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -734,7 +740,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
@@ -742,7 +748,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>19</v>
@@ -764,7 +770,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
@@ -786,13 +792,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -800,13 +806,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -820,7 +826,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -834,7 +840,7 @@
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up shopplinng list function
</commit_message>
<xml_diff>
--- a/data/meals.xlsx
+++ b/data/meals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB6BC99-11FA-4266-B405-31C5D74407AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C8763-C8D3-41CD-B557-EF4F008A16B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>flour, egg, milk,</t>
   </si>
   <si>
-    <t>fiskeboller, potato, carrots,</t>
-  </si>
-  <si>
     <t>paprika, carrot, potato, onion,</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>veggies,</t>
+  </si>
+  <si>
+    <t>fiskeboller, potato, carrot,</t>
   </si>
 </sst>
 </file>
@@ -530,58 +530,58 @@
   <dimension ref="A1:AP20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="3"/>
-    <col min="2" max="2" width="16.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" style="3"/>
+    <col min="2" max="2" width="16.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="3"/>
-    <col min="8" max="8" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" style="3"/>
-    <col min="14" max="14" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" style="3"/>
-    <col min="20" max="20" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" style="3"/>
-    <col min="26" max="26" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.42578125" style="3"/>
-    <col min="32" max="32" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.42578125" style="3"/>
-    <col min="38" max="38" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="16384" width="16.42578125" style="3"/>
+    <col min="5" max="5" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" style="3"/>
+    <col min="8" max="8" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.44140625" style="3"/>
+    <col min="14" max="14" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.44140625" style="3"/>
+    <col min="20" max="20" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.44140625" style="3"/>
+    <col min="26" max="26" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.44140625" style="3"/>
+    <col min="32" max="32" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.44140625" style="3"/>
+    <col min="38" max="38" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="16.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,7 +595,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -630,7 +630,7 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
     </row>
-    <row r="2" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -641,10 +641,10 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -655,54 +655,54 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -713,10 +713,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -727,18 +727,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -749,21 +749,21 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:42" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
@@ -774,18 +774,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -796,21 +796,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -821,10 +821,10 @@
         <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -835,10 +835,10 @@
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -849,18 +849,18 @@
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added summer winter filter
</commit_message>
<xml_diff>
--- a/data/meals.xlsx
+++ b/data/meals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\Documents\Projects\coding\python\meal_planner\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C8763-C8D3-41CD-B557-EF4F008A16B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2D946F-9ECB-4105-ABAC-15E994F51217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t>recipe_name</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>fiskeboller, potato, carrot,</t>
+  </si>
+  <si>
+    <t>season</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>summer</t>
   </si>
 </sst>
 </file>
@@ -530,8 +542,8 @@
   <dimension ref="A1:AP20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,7 +553,7 @@
     <col min="3" max="3" width="20.44140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.44140625" style="3"/>
     <col min="8" max="8" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
@@ -597,7 +609,9 @@
       <c r="E1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -643,6 +657,9 @@
       <c r="D2" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -654,6 +671,9 @@
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F3" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -665,6 +685,9 @@
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -676,6 +699,9 @@
       <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -687,6 +713,9 @@
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F6" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -701,6 +730,9 @@
       <c r="D7" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -715,6 +747,9 @@
       <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -726,6 +761,9 @@
       <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="10" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -737,8 +775,11 @@
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -750,6 +791,9 @@
       </c>
       <c r="D11" s="3" t="s">
         <v>35</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
@@ -762,6 +806,9 @@
       <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="13" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -773,6 +820,9 @@
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -784,8 +834,11 @@
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="F14" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
@@ -794,6 +847,9 @@
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
@@ -809,8 +865,11 @@
       <c r="E16" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -823,8 +882,11 @@
       <c r="E17" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -837,8 +899,11 @@
       <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F18" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -851,8 +916,11 @@
       <c r="D19" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>51</v>
       </c>
@@ -861,6 +929,9 @@
       </c>
       <c r="D20" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>